<commit_message>
commit change version lavarel
</commit_message>
<xml_diff>
--- a/docs/A100.xlsx
+++ b/docs/A100.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="6420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="6420" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ThongTinSanPham" sheetId="2" r:id="rId1"/>
-    <sheet name="ThongTinLienHe" sheetId="3" r:id="rId2"/>
-    <sheet name="BaiGioiThieu" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId2"/>
+    <sheet name="ThongTinLienHe" sheetId="3" r:id="rId3"/>
+    <sheet name="BaiGioiThieu" sheetId="4" r:id="rId4"/>
+    <sheet name="Common" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="95">
   <si>
     <t>Tên sản phẩm</t>
   </si>
@@ -104,13 +107,1648 @@
   </si>
   <si>
     <t>https://sofaphucuong.com/gioi-thieu.html</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>productKey</t>
+  </si>
+  <si>
+    <t>nameProduct</t>
+  </si>
+  <si>
+    <t>nameProductEN</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>percentSalePrice</t>
+  </si>
+  <si>
+    <t>pathProduct</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;bigIncrements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>Incrementing ID using a "big integer" equivalent.</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;bigInteger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'votes'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>BIGINT equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;binary</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'data'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>BLOB equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;boolean</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'confirmed'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>BOOLEAN equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;char</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'name'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFDA564A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>CHAR equivalent with a length</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;date</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'created_at'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>DATE equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;dateTime</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'created_at'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>DATETIME equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;decimal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'amount'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFDA564A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFDA564A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>DECIMAL equivalent with a precision and scale</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;double</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'column'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFDA564A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFDA564A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>DOUBLE equivalent with precision, 15 digits in total and 8 after the decimal point</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;enum</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'choices'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0077AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>array</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'foo'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'bar'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>));</t>
+    </r>
+  </si>
+  <si>
+    <t>ENUM equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;float</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'amount'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>FLOAT equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;increments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'id'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>Incrementing ID to the table (primary key).</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;integer</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'votes'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>INTEGER equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;longText</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'description'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>LONGTEXT equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;mediumInteger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'numbers'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>MEDIUMINT equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;mediumText</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'description'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>MEDIUMTEXT equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;morphs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'taggable'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Adds INTEGER </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>taggable_id</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> and STRING </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>taggable_type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;nullableTimestamps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Same as </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>timestamps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, except allows NULLs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;smallInteger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'votes'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>SMALLINT equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;tinyInteger</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'numbers'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>TINYINT equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;softDeletes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Adds </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>deleted_at</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> column for soft deletes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'email'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>VARCHAR equivalent column</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;string</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'name'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFDA564A"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>100</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>VARCHAR equivalent with a length</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;text</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'description'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>TEXT equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'sunrise'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>TIME equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;timestamp</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF2E7D32"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>'added_on'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>);</t>
+    </r>
+  </si>
+  <si>
+    <t>TIMESTAMP equivalent to the table</t>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;timestamps</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Adds </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>created_at</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>updated_at</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>columns</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>$table</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF555555"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>-&gt;rememberToken</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>();</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Adds </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FFF4645F"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>remember_token</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF525252"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> as VARCHAR(100) NULL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>-&gt;nullable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <t>Designate that the column allows NULL values</t>
+  </si>
+  <si>
+    <r>
+      <t>-&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF0077AA"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>(</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF4EA1DF"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>$value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Declare a default value for a column</t>
+  </si>
+  <si>
+    <r>
+      <t>-&gt;unsigned</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF999999"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>()</t>
+    </r>
+  </si>
+  <si>
+    <t>Set INTEGER to UNSIGNED</t>
+  </si>
+  <si>
+    <t>typeProductId</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +1764,71 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF525252"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFF4645F"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF4EA1DF"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF555555"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF999999"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF2E7D32"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FFDA564A"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF0077AA"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF525252"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -146,8 +1847,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -170,12 +1877,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDEE0DF"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDEE0DF"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDEE0DF"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDEE0DF"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -190,6 +1912,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -206,6 +1938,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="car routes table"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="609600" y="8972550"/>
+          <a:ext cx="7105650" cy="3219450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -473,8 +2265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B5:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,7 +2515,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:H12"/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D4:G12"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
@@ -797,7 +2601,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:D5"/>
   <sheetViews>
@@ -826,4 +2630,368 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:C32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="42" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="D3:E12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="5.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="23.42578125" customWidth="1"/>
+    <col min="5" max="5" width="22.5703125" customWidth="1"/>
+    <col min="6" max="6" width="34.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="4:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" spans="4:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="4:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="D9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D10" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>